<commit_message>
Complete project upload to GitHub
</commit_message>
<xml_diff>
--- a/server/users.xlsx
+++ b/server/users.xlsx
@@ -397,9 +397,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -424,47 +424,87 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>21</v>
+        <v>30</v>
       </c>
       <c r="B2" t="str">
-        <v>ss</v>
+        <v>vvvv</v>
       </c>
       <c r="C2" t="str">
-        <v>ss@gmail.com</v>
+        <v>vvvv@gmail.com</v>
       </c>
       <c r="D2" t="str">
         <v>student</v>
       </c>
       <c r="E2" t="str">
-        <v>19/1/2026</v>
+        <v>20/1/2026</v>
       </c>
       <c r="F2" t="str">
-        <v>12:23:22 pm</v>
+        <v>6:28:59 pm</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
+        <v>21</v>
+      </c>
+      <c r="B3" t="str">
+        <v>ss</v>
+      </c>
+      <c r="C3" t="str">
+        <v>ss@gmail.com</v>
+      </c>
+      <c r="D3" t="str">
+        <v>student</v>
+      </c>
+      <c r="E3" t="str">
+        <v>19/1/2026</v>
+      </c>
+      <c r="F3" t="str">
+        <v>12:23:22 pm</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4">
         <v>5</v>
       </c>
-      <c r="B3" t="str">
+      <c r="B4" t="str">
         <v>vasu</v>
       </c>
-      <c r="C3" t="str">
+      <c r="C4" t="str">
         <v>vasu@gmail.com</v>
       </c>
-      <c r="D3" t="str">
+      <c r="D4" t="str">
         <v>admin</v>
       </c>
-      <c r="E3" t="str">
+      <c r="E4" t="str">
         <v>12/1/2026</v>
       </c>
-      <c r="F3" t="str">
+      <c r="F4" t="str">
         <v>2:04:07 pm</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5">
+        <v>33</v>
+      </c>
+      <c r="B5" t="str">
+        <v>aa</v>
+      </c>
+      <c r="C5" t="str">
+        <v>aa@gmail.com</v>
+      </c>
+      <c r="D5" t="str">
+        <v>student</v>
+      </c>
+      <c r="E5" t="str">
+        <v>27/1/2026</v>
+      </c>
+      <c r="F5" t="str">
+        <v>11:31:50 am</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F5"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Final project update - all files included
</commit_message>
<xml_diff>
--- a/server/users.xlsx
+++ b/server/users.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -424,47 +424,47 @@
     </row>
     <row r="2">
       <c r="A2">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="B2" t="str">
-        <v>vvvv</v>
+        <v>ss</v>
       </c>
       <c r="C2" t="str">
-        <v>vvvv@gmail.com</v>
+        <v>ss@gmail.com</v>
       </c>
       <c r="D2" t="str">
         <v>student</v>
       </c>
       <c r="E2" t="str">
-        <v>20/1/2026</v>
+        <v>12/2/2026</v>
       </c>
       <c r="F2" t="str">
-        <v>6:28:59 pm</v>
+        <v>5:20:17 pm</v>
       </c>
     </row>
     <row r="3">
       <c r="A3">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="B3" t="str">
-        <v>ss</v>
+        <v>vv</v>
       </c>
       <c r="C3" t="str">
-        <v>ss@gmail.com</v>
+        <v>vv@gmail.com</v>
       </c>
       <c r="D3" t="str">
         <v>student</v>
       </c>
       <c r="E3" t="str">
-        <v>19/1/2026</v>
+        <v>12/2/2026</v>
       </c>
       <c r="F3" t="str">
-        <v>12:23:22 pm</v>
+        <v>5:17:35 pm</v>
       </c>
     </row>
     <row r="4">
       <c r="A4">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="B4" t="str">
         <v>vasu</v>
@@ -476,35 +476,75 @@
         <v>admin</v>
       </c>
       <c r="E4" t="str">
-        <v>12/1/2026</v>
+        <v>12/2/2026</v>
       </c>
       <c r="F4" t="str">
-        <v>2:04:07 pm</v>
+        <v>5:17:00 pm</v>
       </c>
     </row>
     <row r="5">
       <c r="A5">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="B5" t="str">
-        <v>aa</v>
+        <v>vasu</v>
       </c>
       <c r="C5" t="str">
-        <v>aa@gmail.com</v>
+        <v>vasuu@gmail.com</v>
       </c>
       <c r="D5" t="str">
         <v>student</v>
       </c>
       <c r="E5" t="str">
-        <v>27/1/2026</v>
+        <v>17/2/2026</v>
       </c>
       <c r="F5" t="str">
-        <v>11:31:50 am</v>
+        <v>5:54:19 pm</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6" t="str">
+        <v>vd</v>
+      </c>
+      <c r="C6" t="str">
+        <v>vd@gmail.com</v>
+      </c>
+      <c r="D6" t="str">
+        <v>student</v>
+      </c>
+      <c r="E6" t="str">
+        <v>18/2/2026</v>
+      </c>
+      <c r="F6" t="str">
+        <v>10:29:25 am</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7">
+        <v>11</v>
+      </c>
+      <c r="B7" t="str">
+        <v>John Doe</v>
+      </c>
+      <c r="C7" t="str">
+        <v>john@example.com</v>
+      </c>
+      <c r="D7" t="str">
+        <v>student</v>
+      </c>
+      <c r="E7" t="str">
+        <v>18/2/2026</v>
+      </c>
+      <c r="F7" t="str">
+        <v>10:32:22 am</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F5"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F7"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>